<commit_message>
verified that probe config has no impact
</commit_message>
<xml_diff>
--- a/data/geometry.xlsx
+++ b/data/geometry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="900" windowWidth="20370" windowHeight="13020" tabRatio="839"/>
+    <workbookView xWindow="2325" yWindow="900" windowWidth="20370" windowHeight="13020" tabRatio="839" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations Rough Input" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="92">
   <si>
     <t>Sheet Name</t>
   </si>
@@ -269,6 +269,39 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>p7</t>
+  </si>
+  <si>
+    <t>p8</t>
+  </si>
+  <si>
+    <t>p9</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>p11</t>
   </si>
 </sst>
 </file>
@@ -623,7 +656,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1042,14 +1075,254 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
+        <v>210</v>
+      </c>
+      <c r="G2" s="3">
+        <f>'Calculations Rough Input'!D3/2</f>
+        <v>3.9413323003157918</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <f>H2</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <f>D2</f>
+        <v>1.2</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>210</v>
+      </c>
+      <c r="G3" s="3">
+        <f>G2</f>
+        <v>3.9413323003157918</v>
+      </c>
+      <c r="H3" s="3">
+        <f>H2</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <f>I2</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <f>J2</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <f>K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:D5" si="0">D3</f>
+        <v>1.2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <f>D5+2.5</f>
+        <v>3.7</v>
+      </c>
+      <c r="F6" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <f>D6</f>
+        <v>3.7</v>
+      </c>
+      <c r="F7" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ref="D8:D9" si="1">D7</f>
+        <v>3.7</v>
+      </c>
+      <c r="F8" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <f>D9+2.5</f>
+        <v>6.2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="3">
+        <f>D10</f>
+        <v>6.2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3">
+        <f>D11</f>
+        <v>6.2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1060,7 +1333,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection sqref="A1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>